<commit_message>
resolved 500 error when there is no data in the table
</commit_message>
<xml_diff>
--- a/src/templates/Nursery_Template.xlsx
+++ b/src/templates/Nursery_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\TAD-Reports-BE\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4EEA49-9CEA-4217-8123-53625B2125EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0FC70E-7107-4083-BE5D-6832D148764A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1886" yWindow="1886" windowWidth="30085" windowHeight="14365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="583" yWindow="1843" windowWidth="31723" windowHeight="14366" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
     <t>Regional Office _____________</t>
   </si>
   <si>
-    <t xml:space="preserve"> This is a sample data </t>
+    <t>Delete this sample data before proceeding.</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
protected template headers, updated pmsurvived
</commit_message>
<xml_diff>
--- a/src/templates/Nursery_Template.xlsx
+++ b/src/templates/Nursery_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\TAD-Reports-BE\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A44126-996F-48A3-8AE5-1A7245E2FD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054791ED-B59A-4F0B-8A2A-44A351924318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Region</t>
   </si>
@@ -110,13 +110,16 @@
   </si>
   <si>
     <t>Delete this sample data before proceeding.</t>
+  </si>
+  <si>
+    <t>Nursery Upload Form</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -155,6 +158,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -182,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -205,33 +215,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,210 +497,212 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="15" style="2" customWidth="1"/>
-    <col min="4" max="8" width="20" style="2" customWidth="1"/>
-    <col min="9" max="9" width="40" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20" style="2" customWidth="1"/>
-    <col min="12" max="13" width="15" style="2" customWidth="1"/>
-    <col min="14" max="14" width="30" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="12.53515625" style="2"/>
+    <col min="1" max="3" width="15" style="3" customWidth="1"/>
+    <col min="4" max="8" width="20" style="3" customWidth="1"/>
+    <col min="9" max="9" width="40" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15" style="3" customWidth="1"/>
+    <col min="11" max="11" width="20" style="3" customWidth="1"/>
+    <col min="12" max="13" width="15" style="3" customWidth="1"/>
+    <col min="14" max="14" width="30" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="12.53515625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="10" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="10" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="10" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-    </row>
     <row r="6" spans="1:14" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A6" s="5">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A7" s="5">
         <v>45030</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J7" s="5">
         <v>44516</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K7" s="6">
         <v>10</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M7" s="6">
         <v>2024</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-    </row>
     <row r="8" spans="1:14" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:14" ht="14.6" x14ac:dyDescent="0.4">
@@ -695,7 +737,7 @@
       <c r="M10" s="8"/>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="8"/>
@@ -711,7 +753,7 @@
       <c r="M11" s="8"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="8"/>
@@ -727,7 +769,7 @@
       <c r="M12" s="8"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="8"/>
@@ -824,19 +866,19 @@
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1207,11 +1249,29 @@
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
     </row>
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <sheetProtection algorithmName="SHA-512" hashValue="K/TnSF3qtUX+YmmMtg/UrfUNmIToG2fQn7hvr0d535U5QsHllhGf/ZmR/N56yinYVFF+SjJOBAc0RXv0MJrjXg==" saltValue="wszpPPNHk9gCszHS2FvgWw==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="4">
     <mergeCell ref="E1:L1"/>
     <mergeCell ref="E2:L2"/>
     <mergeCell ref="E3:L3"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>